<commit_message>
unittest data simulation using pickle
</commit_message>
<xml_diff>
--- a/tests/interpolation_results.xlsx
+++ b/tests/interpolation_results.xlsx
@@ -438,7 +438,7 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>0.07550669680654888</v>
+        <v>0.3775334493306695</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -455,7 +455,7 @@
         <v>8</v>
       </c>
       <c r="D3">
-        <v>0.05529756298025576</v>
+        <v>0.2764878078561827</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -472,7 +472,7 @@
         <v>8</v>
       </c>
       <c r="D4">
-        <v>0.06590551671615402</v>
+        <v>0.3295275739855658</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -489,7 +489,7 @@
         <v>7</v>
       </c>
       <c r="D5">
-        <v>0.04864342705756943</v>
+        <v>0.2432171196402437</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -506,7 +506,7 @@
         <v>7</v>
       </c>
       <c r="D6">
-        <v>0.04568188096500522</v>
+        <v>0.228409391030088</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -523,7 +523,7 @@
         <v>8</v>
       </c>
       <c r="D7">
-        <v>0.03905669699612921</v>
+        <v>0.1952834540174026</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
@@ -540,7 +540,7 @@
         <v>8</v>
       </c>
       <c r="D8">
-        <v>0.0434250811625911</v>
+        <v>0.2171253679562946</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
@@ -557,7 +557,7 @@
         <v>7</v>
       </c>
       <c r="D9">
-        <v>0.05019543912139926</v>
+        <v>0.2509771789656824</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
@@ -574,7 +574,7 @@
         <v>8</v>
       </c>
       <c r="D10">
-        <v>0.4279036563066952</v>
+        <v>2.139517179104654</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>

</xml_diff>